<commit_message>
Updated sizes assessment and sized minimum workshop footprint
</commit_message>
<xml_diff>
--- a/Workshop/Size assessment/Size Analysis.xlsx
+++ b/Workshop/Size assessment/Size Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Burgeson\Desktop\gitrepos\velocity\Workshop\Size assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paubur\Documents\gitrepos\velocity\Workshop\Size assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90130F7-AB01-492F-8CB2-8DECD6BD7F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCD8E50-89C1-45AE-904E-C4501FB06142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FF5B7AA4-E009-4CBE-9F08-201AC053F4DB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{FF5B7AA4-E009-4CBE-9F08-201AC053F4DB}"/>
   </bookViews>
   <sheets>
     <sheet name="FuselageTop" sheetId="2" r:id="rId1"/>
@@ -146,12 +146,54 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="23">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -173,12 +215,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -253,7 +289,7 @@
             <c:numRef>
               <c:f>FuselageTop!$C$2:$C$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>-6.2256577619271951</c:v>
@@ -328,7 +364,7 @@
             <c:numRef>
               <c:f>FuselageTop!$D$2:$D$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>4.4734203620214004</c:v>
@@ -438,7 +474,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -500,7 +536,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -551,6 +587,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -558,7 +595,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -855,6 +891,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -862,7 +899,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -987,7 +1023,7 @@
             <c:numRef>
               <c:f>'Right Conard'!$C$2:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.8682457438934108</c:v>
@@ -1008,7 +1044,7 @@
             <c:numRef>
               <c:f>'Right Conard'!$D$2:$D$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.69985196150999407</c:v>
@@ -1064,7 +1100,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1126,7 +1162,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1177,6 +1213,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1184,7 +1221,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1481,6 +1517,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1488,7 +1525,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4143,12 +4179,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A5ABD15-0BD2-4E7F-A1F8-5BE311DE078C}" name="FuselageTop" displayName="FuselageTop" ref="A1:D24" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A1:D23" xr:uid="{8A5ABD15-0BD2-4E7F-A1F8-5BE311DE078C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98707255-BE2F-4F14-8B78-5048E5379786}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{1E8D6016-EE96-4EF2-A535-279C9E18A9CD}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{120C2263-07E3-4C5A-AA20-353DABC8FC14}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{98707255-BE2F-4F14-8B78-5048E5379786}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1E8D6016-EE96-4EF2-A535-279C9E18A9CD}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{120C2263-07E3-4C5A-AA20-353DABC8FC14}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A23146A0-BB19-48E0-9D22-94D6724637AD}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{A23146A0-BB19-48E0-9D22-94D6724637AD}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4157,15 +4193,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3058C0B-256D-48C3-995A-3F545B6D8FD2}" name="Right_Wing" displayName="Right_Wing" ref="A1:D8" tableType="queryTable" totalsRowCount="1" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3058C0B-256D-48C3-995A-3F545B6D8FD2}" name="Right_Wing" displayName="Right_Wing" ref="A1:D8" tableType="queryTable" totalsRowCount="1" dataDxfId="22">
   <autoFilter ref="A1:D7" xr:uid="{A3058C0B-256D-48C3-995A-3F545B6D8FD2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C30A36BE-9FB9-40D0-B379-3B40801541E1}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B49DDCF9-4B6D-4EAC-9E69-FBEABA014949}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{7DCB9BE5-FACF-4AC6-8810-6912EFB813AD}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{C30A36BE-9FB9-40D0-B379-3B40801541E1}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B49DDCF9-4B6D-4EAC-9E69-FBEABA014949}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{7DCB9BE5-FACF-4AC6-8810-6912EFB813AD}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="19">
       <calculatedColumnFormula>Right_Wing[[#This Row],[X Coor]]-Right_Wing[[#Totals],[X Coor]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{70398055-E4BD-4F92-A7FC-32BF96E93413}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{70398055-E4BD-4F92-A7FC-32BF96E93413}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="18">
       <calculatedColumnFormula>Right_Wing[[#This Row],[Y Coor]]-Right_Wing[[#Totals],[Y Coor]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4177,12 +4213,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{925486B1-43A5-441A-A695-933DB56209A6}" name="Right_Conard" displayName="Right_Conard" ref="A1:D6" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A1:D5" xr:uid="{925486B1-43A5-441A-A695-933DB56209A6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A6AECBF3-D5AA-4AD7-A136-3BD3FD26F818}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{04AA9599-D41F-4A3C-AB45-E8E40FCE2546}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{554402FA-AE03-4305-8E0F-48AB28D9BA50}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{A6AECBF3-D5AA-4AD7-A136-3BD3FD26F818}" uniqueName="1" name="X Coor" totalsRowFunction="average" queryTableFieldId="1" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{04AA9599-D41F-4A3C-AB45-E8E40FCE2546}" uniqueName="2" name="Y Coor" totalsRowFunction="average" queryTableFieldId="2" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{554402FA-AE03-4305-8E0F-48AB28D9BA50}" uniqueName="3" name="X Center" queryTableFieldId="3" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>Right_Conard[[#This Row],[X Coor]]-Right_Conard[[#Totals],[X Coor]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E24D941-E1AC-4076-B7A9-85C2495BE52B}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{8E24D941-E1AC-4076-B7A9-85C2495BE52B}" uniqueName="4" name="Y Center" queryTableFieldId="4" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>Right_Conard[[#This Row],[Y Coor]]-Right_Conard[[#Totals],[Y Coor]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4196,10 +4232,10 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2A9D0347-6319-4A75-9680-19037591081A}" uniqueName="1" name="X Coor" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{0F8608A4-1848-4F2A-BE48-6BA01A38A641}" uniqueName="2" name="Y Coor" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{1B0D7EE8-F396-4603-A4D0-E0C57D780FD1}" uniqueName="3" name="X Adj" queryTableFieldId="3" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{1B0D7EE8-F396-4603-A4D0-E0C57D780FD1}" uniqueName="3" name="X Adj" queryTableFieldId="3" dataDxfId="17">
       <calculatedColumnFormula>FueselageSide[[#This Row],[X Coor]]-A$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BA98D9B3-0C18-49A8-B6C7-643E00F7322F}" uniqueName="4" name="Y Adj" queryTableFieldId="4" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{BA98D9B3-0C18-49A8-B6C7-643E00F7322F}" uniqueName="4" name="Y Adj" queryTableFieldId="4" dataDxfId="16">
       <calculatedColumnFormula>FueselageSide[[#This Row],[Y Coor]]-B$7</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4526,16 +4562,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14D75E3-2533-4917-A73D-DE805A0DC1B0}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4549,369 +4586,371 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>28.315321983715762</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>17.139995567514156</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-6.2256577619271951</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>4.4734203620214004</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>32.698001480384896</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>17.117049601563007</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-1.8429782652580613</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>4.450474396070252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>33.317542561065878</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>19.939403413554125</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-1.2234371845770795</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>7.2728282080613695</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>31.665433012583268</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>20.490106596381658</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-2.8755467330596893</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>7.8235313908889026</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>34.556624722427834</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>21.683296825841317</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.5644976784876974E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>9.0167216203485623</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>37.401924500370093</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>20.490106596381658</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>2.8609447547271358</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>7.8235313908889026</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>35.795706883789784</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>19.893511481651831</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.2547271381468263</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>7.2269362761590763</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>36.392301998519613</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>17.094103635611855</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.8513222528766562</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>4.4275284301191</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>40.797927461139899</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>17.139995567514156</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>6.256947715496942</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>4.4734203620214004</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>40.797927461139899</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>15.441994087129254</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>6.256947715496942</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>2.7754188816364991</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
         <v>36.66765358993338</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>10.072638054560786</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>2.1266738442904227</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-2.5939371509319695</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>36.346410066617317</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>7.4109060042277024</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.8054303209743594</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-5.2556692012650528</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>42.312361213915615</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>7.640365663739173</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>7.7713814682726579</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-5.0262095417535821</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>41.991117690599552</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>7.4501379449565945</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-6.7701029540407758</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>35.88749074759437</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.3465110019514128</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-6.7701029540407758</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>34.556624722427834</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>3.0052805416074184</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>1.5644976784876974E-2</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-9.6612946638853359</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>33.225758697261284</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-1.3152210483816731</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-6.7701029540407758</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>26.800888230940043</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-7.7400915147029146</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-6.7701029540407758</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>26.800888230940043</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>7.640365663739173</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-7.7400915147029146</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-5.0262095417535821</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>32.766839378238338</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>7.4109060042277024</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-1.7741403674046197</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-5.2556692012650528</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>32.445595854922274</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>10.072638054560786</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-2.095383890720683</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>-2.5939371509319695</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>28.361213915618059</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>15.396102155226963</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <f>FuselageTop[[#This Row],[X Coor]]-FuselageTop[[#Totals],[X Coor]]</f>
         <v>-6.1797658300248983</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <f>FuselageTop[[#This Row],[Y Coor]]-FuselageTop[[#Totals],[Y Coor]]</f>
         <v>2.7295269497342076</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
         <f>SUBTOTAL(101,FuselageTop[X Coor])</f>
         <v>34.540979745642957</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <f>SUBTOTAL(101,FuselageTop[Y Coor])</f>
         <v>12.666575205492755</v>
       </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -4923,7 +4962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -4935,7 +4974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -4947,7 +4986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -4972,16 +5011,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6056D8-D0AC-4EB1-B928-AD7A36BDA1D4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4995,7 +5034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>19.136935603256848</v>
       </c>
@@ -5011,7 +5050,7 @@
         <v>4.6121391561806107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>19.136935603256848</v>
       </c>
@@ -5027,7 +5066,7 @@
         <v>1.3538119911176913</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>28.315321983715762</v>
       </c>
@@ -5043,7 +5082,7 @@
         <v>-3.1894892672094723</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>28.361213915618059</v>
       </c>
@@ -5059,7 +5098,7 @@
         <v>-1.5373797187268714</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>32.720947446336048</v>
       </c>
@@ -5075,7 +5114,7 @@
         <v>-1.4914877868245711</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>33.088082901554401</v>
       </c>
@@ -5091,7 +5130,7 @@
         <v>0.25240562546262169</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>SUBTOTAL(101,Right_Wing[X Coor])</f>
         <v>26.793239575622994</v>
@@ -5101,7 +5140,7 @@
         <v>18.631483354338727</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -5113,7 +5152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -5138,16 +5177,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA5C2C9-E8BE-4315-82A2-5AFC6F1BECAF}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5161,81 +5200,83 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>32.766839378238338</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>7.4109060042277024</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>Right_Conard[[#This Row],[X Coor]]-Right_Conard[[#Totals],[X Coor]]</f>
         <v>2.8682457438934108</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>Right_Conard[[#This Row],[Y Coor]]-Right_Conard[[#Totals],[Y Coor]]</f>
         <v>0.69985196150999407</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>26.800888230940043</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>7.640365663739173</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>Right_Conard[[#This Row],[X Coor]]-Right_Conard[[#Totals],[X Coor]]</f>
         <v>-3.0977054034048841</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>Right_Conard[[#This Row],[Y Coor]]-Right_Conard[[#Totals],[Y Coor]]</f>
         <v>0.9293116210214647</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>26.800888230940043</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>Right_Conard[[#This Row],[X Coor]]-Right_Conard[[#Totals],[X Coor]]</f>
         <v>-3.0977054034048841</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>Right_Conard[[#This Row],[Y Coor]]-Right_Conard[[#Totals],[Y Coor]]</f>
         <v>-0.81458179126572894</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>33.225758697261284</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5.8964722514519794</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>Right_Conard[[#This Row],[X Coor]]-Right_Conard[[#Totals],[X Coor]]</f>
         <v>3.3271650629163574</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f>Right_Conard[[#This Row],[Y Coor]]-Right_Conard[[#Totals],[Y Coor]]</f>
         <v>-0.81458179126572894</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <f>SUBTOTAL(101,Right_Conard[X Coor])</f>
         <v>29.898593634344927</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <f>SUBTOTAL(101,Right_Conard[Y Coor])</f>
         <v>6.7110540427177083</v>
       </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -5247,7 +5288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -5272,16 +5313,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC88DF-5C52-482B-A076-DB97DAAED01E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5295,7 +5336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>131.29411764705881</v>
       </c>
@@ -5311,7 +5352,7 @@
         <v>54.529411764705856</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>231.35294117647055</v>
       </c>
@@ -5327,7 +5368,7 @@
         <v>66.705882352941174</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>317.11764705882354</v>
       </c>
@@ -5343,7 +5384,7 @@
         <v>43.147058823529392</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>214.41176470588232</v>
       </c>
@@ -5359,7 +5400,7 @@
         <v>26.999999999999986</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>292.76470588235293</v>
       </c>
@@ -5375,7 +5416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>186.75</v>
       </c>
@@ -5391,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>